<commit_message>
Fixed all errors for script
</commit_message>
<xml_diff>
--- a/Put on website and attach id.xlsb.xlsx
+++ b/Put on website and attach id.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gocreate-filling-website-script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597B0FA3-697E-40F3-BD2E-C188E0C9853C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080ADC0E-214C-4244-BE88-0766B24A35B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{7B60883F-7493-497D-98A5-055017696140}"/>
+    <workbookView xWindow="1868" yWindow="1020" windowWidth="14467" windowHeight="9533" xr2:uid="{7B60883F-7493-497D-98A5-055017696140}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,13 +251,13 @@
     <t>scripttest2</t>
   </si>
   <si>
-    <t>scriptttest4</t>
-  </si>
-  <si>
     <t>scripttest3</t>
   </si>
   <si>
-    <t>cripttest3@email.com</t>
+    <t>scripttest4</t>
+  </si>
+  <si>
+    <t>testscript3@email.com</t>
   </si>
 </sst>
 </file>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA22BC0D-0585-4114-BE36-E316B5DBF9A9}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -869,7 +869,7 @@
         <v>76</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>46</v>
@@ -953,7 +953,7 @@
         <v>71</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>59</v>

</xml_diff>